<commit_message>
Added scripts to validate the bots generated scripts and save the results. added script to automate prompting the bot based on selected papers search strings
</commit_message>
<xml_diff>
--- a/validation/dataset/final_dataset-June-2023-modified.xlsx
+++ b/validation/dataset/final_dataset-June-2023-modified.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodol\OneDrive\Documents\SE-ALL\SearchStringAI\validation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodol\OneDrive\Documents\SE-ALL\SearchStringAI\validation\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C04321D3-A3DD-498F-BD7F-9C65850FEA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062D7ED8-88C2-4943-B9EC-8621D42AD08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-86" yWindow="0" windowWidth="16629" windowHeight="17880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2044,9 +2044,6 @@
   </si>
   <si>
     <t>(software!) AND (measurement pro*) AND (met* OR evaluat* OR improv* OR goal OR challenge OR problem OR issue OR lessons OR experience OR GQM OR success OR fail OR tool)</t>
-  </si>
-  <si>
-    <t>(“technical debt”)OR (“design debt”) OR (“architect* debt”) OR (“test* debt”) OR (“implem* debt”) OR (“docum* debt”) OR (“requirement debt”) OR (“code debt”) OR (“Infrastructure debt”) OR (“versioning debt”) OR (“defect debt”) OR (“build debt”)</t>
   </si>
   <si>
     <t>(product line OR product family OR system family) AND (confugyration OR product selection OR feature selection) AND (attribute OR non-functional OR quality OR preference OR requirement)</t>
@@ -2429,6 +2426,9 @@
 RQ2: What conclusions can be deducted from the studies found?
 RQ3: How can user experience in Agile software development be planned and controlled for a product backlog item or a requirement before the development?
 RQ4: What retrospective proposals exist to improve the efficiency and effectiveness of the user experience process in terms of Agile software development?</t>
+  </si>
+  <si>
+    <t>(“technical debt”) OR (“design debt”) OR (“architect* debt”) OR (“test* debt”) OR (“implem* debt”) OR (“docum* debt”) OR (“requirement debt”) OR (“code debt”) OR (“Infrastructure debt”) OR (“versioning debt”) OR (“defect debt”) OR (“build debt”)</t>
   </si>
 </sst>
 </file>
@@ -2580,7 +2580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2626,15 +2626,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2942,8 +2933,8 @@
   </sheetPr>
   <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B41" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6"/>
@@ -2982,10 +2973,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="I1" s="5" t="s">
         <v>229</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>230</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>7</v>
@@ -2994,10 +2985,10 @@
         <v>8</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>280</v>
+        <v>262</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="18.75" customHeight="1">
@@ -3961,7 +3952,7 @@
         <v>1</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>223</v>
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="18.75" customHeight="1">
@@ -3993,10 +3984,10 @@
         <v>1</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="18.75" customHeight="1">
@@ -4028,10 +4019,10 @@
         <v>1</v>
       </c>
       <c r="J35" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="K35" s="19" t="s">
         <v>226</v>
-      </c>
-      <c r="K35" s="19" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="18.75" customHeight="1">
@@ -4063,10 +4054,10 @@
         <v>1</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K36" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="18.75" customHeight="1">
@@ -4098,10 +4089,10 @@
         <v>1</v>
       </c>
       <c r="J37" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="K37" s="11" t="s">
         <v>232</v>
-      </c>
-      <c r="K37" s="11" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="38" spans="1:12" ht="18.75" customHeight="1">
@@ -4130,13 +4121,13 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J38" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="K38" t="s">
         <v>234</v>
-      </c>
-      <c r="K38" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="39" spans="1:12" ht="18.75" customHeight="1">
@@ -4168,10 +4159,10 @@
         <v>4</v>
       </c>
       <c r="J39" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="L39" t="s">
         <v>236</v>
-      </c>
-      <c r="L39" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="40" spans="1:12" ht="18.75" customHeight="1">
@@ -4203,13 +4194,13 @@
         <v>1</v>
       </c>
       <c r="J40" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="K40" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="K40" s="6" t="s">
+      <c r="L40" t="s">
         <v>239</v>
-      </c>
-      <c r="L40" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="18.75" customHeight="1">
@@ -4241,10 +4232,10 @@
         <v>1</v>
       </c>
       <c r="J41" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="K41" t="s">
         <v>241</v>
-      </c>
-      <c r="K41" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="18.75" customHeight="1">
@@ -4270,19 +4261,19 @@
         <v>2006</v>
       </c>
       <c r="H42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="K42" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L42" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="18.75" customHeight="1">
@@ -4314,10 +4305,10 @@
         <v>1</v>
       </c>
       <c r="J43" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="K43" s="6" t="s">
         <v>244</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="18.75" customHeight="1">
@@ -4349,10 +4340,10 @@
         <v>1</v>
       </c>
       <c r="J44" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="K44" t="s">
         <v>246</v>
-      </c>
-      <c r="K44" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="45" spans="1:12" ht="18.75" customHeight="1">
@@ -4384,10 +4375,10 @@
         <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="K45" s="6" t="s">
         <v>248</v>
-      </c>
-      <c r="K45" s="6" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="18.75" customHeight="1">
@@ -4416,13 +4407,13 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J46" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="K46" t="s">
         <v>250</v>
-      </c>
-      <c r="K46" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="18.75" customHeight="1">
@@ -4451,10 +4442,10 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="18.75" customHeight="1">
@@ -4486,10 +4477,10 @@
         <v>1</v>
       </c>
       <c r="J48" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="K48" t="s">
         <v>253</v>
-      </c>
-      <c r="K48" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="49" spans="1:13" ht="18.75" customHeight="1">
@@ -4521,10 +4512,10 @@
         <v>1</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="50" spans="1:13" ht="18.75" customHeight="1">
@@ -4556,10 +4547,10 @@
         <v>1</v>
       </c>
       <c r="J50" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="K50" t="s">
         <v>257</v>
-      </c>
-      <c r="K50" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="51" spans="1:13" ht="18.75" customHeight="1">
@@ -4591,10 +4582,10 @@
         <v>1</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="K51" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="52" spans="1:13" ht="18.75" customHeight="1">
@@ -4626,10 +4617,10 @@
         <v>1</v>
       </c>
       <c r="J52" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="K52" s="20" t="s">
         <v>261</v>
-      </c>
-      <c r="K52" s="20" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="18.75" customHeight="1">
@@ -4658,10 +4649,10 @@
         <v>9</v>
       </c>
       <c r="I53" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="54" spans="1:13" ht="18.75" customHeight="1">
@@ -4686,14 +4677,14 @@
       <c r="G54" s="3">
         <v>2011</v>
       </c>
-      <c r="H54" s="21">
+      <c r="H54" s="17">
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="55" spans="1:13" ht="18.75" customHeight="1">
@@ -4718,17 +4709,17 @@
       <c r="G55" s="3">
         <v>2020</v>
       </c>
-      <c r="H55" s="21">
+      <c r="H55" s="17">
         <v>5</v>
       </c>
-      <c r="I55" s="22">
+      <c r="I55" s="9">
         <v>1</v>
       </c>
       <c r="J55" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="K55" t="s">
         <v>266</v>
-      </c>
-      <c r="K55" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="56" spans="1:13" ht="18.75" customHeight="1">
@@ -4753,17 +4744,17 @@
       <c r="G56" s="3">
         <v>2018</v>
       </c>
-      <c r="H56" s="21">
+      <c r="H56" s="17">
         <v>2</v>
       </c>
-      <c r="I56" s="22">
+      <c r="I56" s="9">
         <v>1</v>
       </c>
       <c r="J56" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="K56" t="s">
         <v>268</v>
-      </c>
-      <c r="K56" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="57" spans="1:13" ht="18.75" customHeight="1">
@@ -4788,17 +4779,17 @@
       <c r="G57" s="3">
         <v>2012</v>
       </c>
-      <c r="H57" s="21">
+      <c r="H57" s="17">
         <v>6</v>
       </c>
-      <c r="I57" s="22">
+      <c r="I57" s="9">
         <v>6</v>
       </c>
       <c r="J57" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="K57" s="6" t="s">
         <v>270</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="58" spans="1:13" ht="18.75" customHeight="1">
@@ -4823,17 +4814,17 @@
       <c r="G58" s="3">
         <v>2017</v>
       </c>
-      <c r="H58" s="21">
+      <c r="H58" s="17">
         <v>3</v>
       </c>
-      <c r="I58" s="22">
+      <c r="I58" s="9">
         <v>1</v>
       </c>
       <c r="J58" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="K58" t="s">
         <v>272</v>
-      </c>
-      <c r="K58" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="59" spans="1:13" ht="18.75" customHeight="1">
@@ -4858,17 +4849,17 @@
       <c r="G59" s="3">
         <v>2013</v>
       </c>
-      <c r="H59" s="21">
+      <c r="H59" s="17">
         <v>5</v>
       </c>
-      <c r="I59" s="22">
+      <c r="I59" s="9">
         <v>1</v>
       </c>
       <c r="J59" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="K59" t="s">
         <v>274</v>
-      </c>
-      <c r="K59" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="60" spans="1:13" ht="18.75" customHeight="1">
@@ -4893,17 +4884,17 @@
       <c r="G60" s="3">
         <v>2010</v>
       </c>
-      <c r="H60" s="21">
+      <c r="H60" s="17">
         <v>1</v>
       </c>
-      <c r="I60" s="22">
+      <c r="I60" s="9">
         <v>1</v>
       </c>
       <c r="J60" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="K60" s="6" t="s">
         <v>276</v>
-      </c>
-      <c r="K60" s="6" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="61" spans="1:13" ht="18.75" customHeight="1">
@@ -4928,20 +4919,20 @@
       <c r="G61" s="3">
         <v>2013</v>
       </c>
-      <c r="H61" s="21">
+      <c r="H61" s="17">
         <v>5</v>
       </c>
-      <c r="I61" s="22">
+      <c r="I61" s="9">
         <v>23</v>
       </c>
       <c r="J61" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="K61" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="K61" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="M61" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="62" spans="1:13" ht="18.75" customHeight="1">
@@ -4966,20 +4957,20 @@
       <c r="G62" s="3">
         <v>2019</v>
       </c>
-      <c r="H62" s="21">
+      <c r="H62" s="17">
         <v>4</v>
       </c>
-      <c r="I62" s="22">
+      <c r="I62" s="9">
         <v>1</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M62" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="63" spans="1:13" ht="18.75" customHeight="1">

</xml_diff>

<commit_message>
Fixed dataset typos and updated validation scores
</commit_message>
<xml_diff>
--- a/validation/dataset/final_dataset-June-2023-modified.xlsx
+++ b/validation/dataset/final_dataset-June-2023-modified.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodol\OneDrive\Documents\SE-ALL\SearchStringAI\validation\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062D7ED8-88C2-4943-B9EC-8621D42AD08A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2816B0-8A27-4964-B4CD-47ECADD87E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14871" yWindow="4671" windowWidth="17735" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -630,25 +630,10 @@
     <t>What success factors of CSDO are reported in the existing literature and mention by the experts? Are there any differences between the findings of the literature and the questionnaire survey? What would be the priority of the investigated success factors? How to develop a prioritization-based taxonomy of the identified factors?</t>
   </si>
   <si>
-    <t>("success factors" OR "factors" OR "aspects" OR "items" OR "elements" OR "drivers" OR "motivators" OR "variables")
-AND
-("Outsourcing" OR "global software development" OR "geographically distributed development" OR "offshore development" OR "multisite development" OR "collaborative software development")
-AND
-("IaaS" OR "PaaS" OR "SaaS" OR "XaaS" OR "Infrastructure as a Service" OR "Platform as a Service" OR "Software as a Service" OR "IT service" OR "Application Service" OR "ASP")
-AND
-("cloud computing" OR "cloud platform" OR "cloud provider" OR "cloud service" OR "cloud offering")</t>
-  </si>
-  <si>
     <t>How often are model transformation design patterns used in practice in MT development?Which categories of patterns and which individual patterns are used?Is the use explicit (recognised as a specific design decision) or not? Are different categories of patterns used for particular categories of transformations? What perceived benefits were obtained from using patterns?Is there evidence for these benefits? Are there cases where patterns should have been applied?Are there necessary patterns which have not yet been formalised?  Has there been a change in the adoption of MT patterns over time?Have papers cataloguing MT patterns been influential for MT developers? Do different MT languages differ in their capabilities for expressing and using MT patterns?</t>
   </si>
   <si>
     <t>Model transformation</t>
-  </si>
-  <si>
-    <t>(blockchain OR
-((distributed OR decentralized)
-AND (ledger OR platform OR "autonomous organization")))
-AND (governance OR management OR ecosystem)</t>
   </si>
   <si>
     <t>what is blockchain governance, and what are its building blocks?</t>
@@ -2430,12 +2415,21 @@
   <si>
     <t>(“technical debt”) OR (“design debt”) OR (“architect* debt”) OR (“test* debt”) OR (“implem* debt”) OR (“docum* debt”) OR (“requirement debt”) OR (“code debt”) OR (“Infrastructure debt”) OR (“versioning debt”) OR (“defect debt”) OR (“build debt”)</t>
   </si>
+  <si>
+    <t>("success factors" OR "factors" OR "aspects" OR "items" OR "elements" OR "drivers" OR "motivators" OR "variables") AND ("Outsourcing" OR "global software development" OR "geographically distributed development" OR "offshore development" OR "multisite development" OR "collaborative software development") AND ("IaaS" OR "PaaS" OR "SaaS" OR "XaaS" OR "Infrastructure as a Service" OR "Platform as a Service" OR "Software as a Service" OR "IT service" OR "Application Service" OR "ASP")
+AND
+("cloud computing" OR "cloud platform" OR "cloud provider" OR "cloud service" OR "cloud offering")</t>
+  </si>
+  <si>
+    <t>(blockchain OR ((distributed OR decentralized) AND (ledger OR platform OR "autonomous organization")))
+AND (governance OR management OR ecosystem)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2933,11 +2927,11 @@
   </sheetPr>
   <dimension ref="A1:M171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D30" workbookViewId="0">
-      <selection activeCell="K64" sqref="K64"/>
+    <sheetView tabSelected="1" topLeftCell="D5" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8.53515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="110.84375" bestFit="1" customWidth="1"/>
@@ -2950,7 +2944,7 @@
     <col min="11" max="11" width="13.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2973,10 +2967,10 @@
         <v>6</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J1" s="18" t="s">
         <v>7</v>
@@ -2985,13 +2979,13 @@
         <v>8</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3014,7 +3008,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.75" customHeight="1">
+    <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3043,7 +3037,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.75" customHeight="1">
+    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3078,7 +3072,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18.75" customHeight="1">
+    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3107,7 +3101,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18.75" customHeight="1">
+    <row r="6" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3130,7 +3124,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18.75" customHeight="1">
+    <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3159,7 +3153,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18.75" customHeight="1">
+    <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3191,7 +3185,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.75" customHeight="1">
+    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -3226,7 +3220,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.75" customHeight="1">
+    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -3255,7 +3249,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.75" customHeight="1">
+    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -3287,10 +3281,10 @@
         <v>199</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -3319,13 +3313,13 @@
         <v>1</v>
       </c>
       <c r="J12" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="K12" t="s">
         <v>201</v>
       </c>
-      <c r="K12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1">
+    </row>
+    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3354,13 +3348,13 @@
         <v>1</v>
       </c>
       <c r="J13" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3389,13 +3383,13 @@
         <v>1</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3424,13 +3418,13 @@
         <v>1</v>
       </c>
       <c r="J15" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="18.75" customHeight="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3459,16 +3453,16 @@
         <v>1</v>
       </c>
       <c r="J16" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="L16" t="s">
         <v>209</v>
       </c>
-      <c r="K16" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="L16" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="18.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3494,10 +3488,10 @@
         <v>1</v>
       </c>
       <c r="J17" s="6" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="18.75" customHeight="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3523,10 +3517,10 @@
         <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="18.75" customHeight="1">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3549,7 +3543,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="18.75" customHeight="1">
+    <row r="20" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3572,7 +3566,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="18.75" customHeight="1">
+    <row r="21" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3595,7 +3589,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="18.75" customHeight="1">
+    <row r="22" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3618,7 +3612,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="18.75" customHeight="1">
+    <row r="23" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3641,7 +3635,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="18.75" customHeight="1">
+    <row r="24" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3667,10 +3661,10 @@
         <v>1</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="18.75" customHeight="1">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3696,13 +3690,13 @@
         <v>1</v>
       </c>
       <c r="K25" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L25" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="18.75" customHeight="1">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3731,7 +3725,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="18.75" customHeight="1">
+    <row r="27" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3760,10 +3754,10 @@
         <v>1</v>
       </c>
       <c r="K27" s="10" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="18.75" customHeight="1">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3792,10 +3786,10 @@
         <v>1</v>
       </c>
       <c r="K28" s="11" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="18.75" customHeight="1">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3824,10 +3818,10 @@
         <v>1</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="18.75" customHeight="1">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3856,10 +3850,10 @@
         <v>1</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="18.75" customHeight="1">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3888,10 +3882,10 @@
         <v>1</v>
       </c>
       <c r="K31" s="13" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="18.75" customHeight="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3920,10 +3914,10 @@
         <v>1</v>
       </c>
       <c r="K32" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="18.75" customHeight="1">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3952,10 +3946,10 @@
         <v>1</v>
       </c>
       <c r="K33" s="14" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="18.75" customHeight="1">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -3984,13 +3978,13 @@
         <v>1</v>
       </c>
       <c r="J34" s="6" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K34" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="18.75" customHeight="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -4019,13 +4013,13 @@
         <v>1</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="18.75" customHeight="1">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -4054,13 +4048,13 @@
         <v>1</v>
       </c>
       <c r="J36" s="6" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="K36" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="18.75" customHeight="1">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -4089,13 +4083,13 @@
         <v>1</v>
       </c>
       <c r="J37" s="6" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K37" s="11" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="18.75" customHeight="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -4121,16 +4115,16 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K38" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="18.75" customHeight="1">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -4159,13 +4153,13 @@
         <v>4</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="L39" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" ht="18.75" customHeight="1">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -4194,16 +4188,16 @@
         <v>1</v>
       </c>
       <c r="J40" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="L40" t="s">
         <v>237</v>
       </c>
-      <c r="K40" s="6" t="s">
-        <v>238</v>
-      </c>
-      <c r="L40" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" ht="18.75" customHeight="1">
+    </row>
+    <row r="41" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -4232,13 +4226,13 @@
         <v>1</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K41" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" ht="18.75" customHeight="1">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -4261,22 +4255,22 @@
         <v>2006</v>
       </c>
       <c r="H42" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="I42" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J42" s="6" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="K42" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L42" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" ht="18.75" customHeight="1">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -4305,13 +4299,13 @@
         <v>1</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" ht="18.75" customHeight="1">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -4340,13 +4334,13 @@
         <v>1</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="K44" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" ht="18.75" customHeight="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -4375,13 +4369,13 @@
         <v>1</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" ht="18.75" customHeight="1">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -4407,16 +4401,16 @@
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K46" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="18.75" customHeight="1">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -4442,13 +4436,13 @@
         <v>3</v>
       </c>
       <c r="I47" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" ht="18.75" customHeight="1">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -4477,13 +4471,13 @@
         <v>1</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K48" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" ht="18.75" customHeight="1">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -4512,13 +4506,13 @@
         <v>1</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" ht="18.75" customHeight="1">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -4547,13 +4541,13 @@
         <v>1</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="K50" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" ht="18.75" customHeight="1">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -4582,13 +4576,13 @@
         <v>1</v>
       </c>
       <c r="J51" s="6" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K51" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" ht="18.75" customHeight="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -4617,13 +4611,13 @@
         <v>1</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="K52" s="20" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" ht="18.75" customHeight="1">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -4649,13 +4643,13 @@
         <v>9</v>
       </c>
       <c r="I53" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" ht="18.75" customHeight="1">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3">
         <v>53</v>
       </c>
@@ -4681,13 +4675,13 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" ht="18.75" customHeight="1">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3">
         <v>54</v>
       </c>
@@ -4716,13 +4710,13 @@
         <v>1</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K55" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" ht="18.75" customHeight="1">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3">
         <v>55</v>
       </c>
@@ -4751,13 +4745,13 @@
         <v>1</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K56" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" ht="18.75" customHeight="1">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3">
         <v>56</v>
       </c>
@@ -4786,13 +4780,13 @@
         <v>6</v>
       </c>
       <c r="J57" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" ht="18.75" customHeight="1">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3">
         <v>57</v>
       </c>
@@ -4821,13 +4815,13 @@
         <v>1</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K58" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" ht="18.75" customHeight="1">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3">
         <v>58</v>
       </c>
@@ -4856,13 +4850,13 @@
         <v>1</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="K59" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" ht="18.75" customHeight="1">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3">
         <v>59</v>
       </c>
@@ -4891,13 +4885,13 @@
         <v>1</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="K60" s="6" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" ht="18.75" customHeight="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3">
         <v>60</v>
       </c>
@@ -4926,16 +4920,16 @@
         <v>23</v>
       </c>
       <c r="J61" s="6" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="K61" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="M61" t="s">
         <v>278</v>
       </c>
-      <c r="M61" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" ht="18.75" customHeight="1">
+    </row>
+    <row r="62" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A62" s="3">
         <v>61</v>
       </c>
@@ -4964,16 +4958,16 @@
         <v>1</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="K62" s="6" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M62" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" ht="18.75" customHeight="1">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3">
         <v>62</v>
       </c>
@@ -4996,7 +4990,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18.75" customHeight="1">
+    <row r="64" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3">
         <v>63</v>
       </c>
@@ -5019,7 +5013,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="18.75" customHeight="1">
+    <row r="65" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3">
         <v>64</v>
       </c>
@@ -5042,7 +5036,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="18.75" customHeight="1">
+    <row r="66" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3">
         <v>65</v>
       </c>
@@ -5065,7 +5059,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="18.75" customHeight="1">
+    <row r="67" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A67" s="3">
         <v>66</v>
       </c>
@@ -5088,7 +5082,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="18.75" customHeight="1">
+    <row r="68" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3">
         <v>67</v>
       </c>
@@ -5111,7 +5105,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="18.75" customHeight="1">
+    <row r="69" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3">
         <v>68</v>
       </c>
@@ -5134,7 +5128,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="18.75" customHeight="1">
+    <row r="70" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3">
         <v>69</v>
       </c>
@@ -5157,7 +5151,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="18.75" customHeight="1">
+    <row r="71" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3">
         <v>70</v>
       </c>
@@ -5180,7 +5174,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="18.75" customHeight="1">
+    <row r="72" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3">
         <v>71</v>
       </c>
@@ -5203,7 +5197,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="18.75" customHeight="1">
+    <row r="73" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3">
         <v>72</v>
       </c>
@@ -5226,7 +5220,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="18.75" customHeight="1">
+    <row r="74" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3">
         <v>73</v>
       </c>
@@ -5249,7 +5243,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="18.75" customHeight="1">
+    <row r="75" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3">
         <v>74</v>
       </c>
@@ -5272,7 +5266,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="18.75" customHeight="1">
+    <row r="76" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3">
         <v>75</v>
       </c>
@@ -5295,7 +5289,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="18.75" customHeight="1">
+    <row r="77" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A77" s="3">
         <v>76</v>
       </c>
@@ -5318,7 +5312,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="18.75" customHeight="1">
+    <row r="78" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3">
         <v>77</v>
       </c>
@@ -5341,7 +5335,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="18.75" customHeight="1">
+    <row r="79" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3">
         <v>78</v>
       </c>
@@ -5364,7 +5358,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="18.75" customHeight="1">
+    <row r="80" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3">
         <v>79</v>
       </c>
@@ -5387,7 +5381,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="18.75" customHeight="1">
+    <row r="81" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3">
         <v>80</v>
       </c>
@@ -5410,7 +5404,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="18.75" customHeight="1">
+    <row r="82" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A82" s="3">
         <v>81</v>
       </c>
@@ -5433,7 +5427,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="18.75" customHeight="1">
+    <row r="83" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A83" s="3">
         <v>82</v>
       </c>
@@ -5456,7 +5450,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="18.75" customHeight="1">
+    <row r="84" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3">
         <v>83</v>
       </c>
@@ -5479,7 +5473,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="18.75" customHeight="1">
+    <row r="85" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A85" s="3">
         <v>84</v>
       </c>
@@ -5502,7 +5496,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="18.75" customHeight="1">
+    <row r="86" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3">
         <v>85</v>
       </c>
@@ -5525,7 +5519,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="18.75" customHeight="1">
+    <row r="87" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A87" s="3">
         <v>86</v>
       </c>
@@ -5548,7 +5542,7 @@
         <v>2005</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="18.75" customHeight="1">
+    <row r="88" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3">
         <v>87</v>
       </c>
@@ -5571,7 +5565,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="18.75" customHeight="1">
+    <row r="89" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A89" s="3">
         <v>88</v>
       </c>
@@ -5594,7 +5588,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="18.75" customHeight="1">
+    <row r="90" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A90" s="3">
         <v>89</v>
       </c>
@@ -5617,7 +5611,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="18.75" customHeight="1">
+    <row r="91" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3">
         <v>90</v>
       </c>
@@ -5640,7 +5634,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="18.75" customHeight="1">
+    <row r="92" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3">
         <v>91</v>
       </c>
@@ -5663,7 +5657,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="18.75" customHeight="1">
+    <row r="93" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A93" s="3">
         <v>92</v>
       </c>
@@ -5686,7 +5680,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="18.75" customHeight="1">
+    <row r="94" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A94" s="3">
         <v>93</v>
       </c>
@@ -5709,7 +5703,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="18.75" customHeight="1">
+    <row r="95" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3">
         <v>94</v>
       </c>
@@ -5732,7 +5726,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="18.75" customHeight="1">
+    <row r="96" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A96" s="3">
         <v>95</v>
       </c>
@@ -5755,7 +5749,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="18.75" customHeight="1">
+    <row r="97" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A97" s="3">
         <v>96</v>
       </c>
@@ -5778,7 +5772,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="18.75" customHeight="1">
+    <row r="98" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A98" s="3">
         <v>97</v>
       </c>
@@ -5801,7 +5795,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="18.75" customHeight="1">
+    <row r="99" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A99" s="3">
         <v>98</v>
       </c>
@@ -5824,7 +5818,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="18.75" customHeight="1">
+    <row r="100" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A100" s="3">
         <v>99</v>
       </c>
@@ -5847,7 +5841,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="18.75" customHeight="1">
+    <row r="101" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A101" s="3">
         <v>100</v>
       </c>
@@ -5870,7 +5864,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="18.75" customHeight="1">
+    <row r="102" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A102" s="3">
         <v>101</v>
       </c>
@@ -5893,7 +5887,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="18.75" customHeight="1">
+    <row r="103" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A103" s="3">
         <v>102</v>
       </c>
@@ -5916,7 +5910,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="18.75" customHeight="1">
+    <row r="104" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A104" s="3">
         <v>103</v>
       </c>
@@ -5939,7 +5933,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="18.75" customHeight="1">
+    <row r="105" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A105" s="3">
         <v>104</v>
       </c>
@@ -5962,7 +5956,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="18.75" customHeight="1">
+    <row r="106" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A106" s="3">
         <v>105</v>
       </c>
@@ -5985,7 +5979,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="18.75" customHeight="1">
+    <row r="107" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A107" s="3">
         <v>106</v>
       </c>
@@ -6008,7 +6002,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="18.75" customHeight="1">
+    <row r="108" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A108" s="3">
         <v>107</v>
       </c>
@@ -6031,7 +6025,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="18.75" customHeight="1">
+    <row r="109" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A109" s="3">
         <v>108</v>
       </c>
@@ -6054,7 +6048,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="18.75" customHeight="1">
+    <row r="110" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A110" s="3">
         <v>109</v>
       </c>
@@ -6077,7 +6071,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="18.75" customHeight="1">
+    <row r="111" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A111" s="3">
         <v>110</v>
       </c>
@@ -6100,7 +6094,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="18.75" customHeight="1">
+    <row r="112" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A112" s="3">
         <v>111</v>
       </c>
@@ -6123,7 +6117,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="18.75" customHeight="1">
+    <row r="113" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A113" s="3">
         <v>112</v>
       </c>
@@ -6146,7 +6140,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="18.75" customHeight="1">
+    <row r="114" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A114" s="3">
         <v>113</v>
       </c>
@@ -6169,7 +6163,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="115" spans="1:7" ht="18.75" customHeight="1">
+    <row r="115" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A115" s="3">
         <v>114</v>
       </c>
@@ -6192,7 +6186,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="116" spans="1:7" ht="18.75" customHeight="1">
+    <row r="116" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A116" s="3">
         <v>115</v>
       </c>
@@ -6215,7 +6209,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="18.75" customHeight="1">
+    <row r="117" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A117" s="3">
         <v>116</v>
       </c>
@@ -6238,7 +6232,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="118" spans="1:7" ht="18.75" customHeight="1">
+    <row r="118" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A118" s="3">
         <v>117</v>
       </c>
@@ -6261,7 +6255,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="119" spans="1:7" ht="18.75" customHeight="1">
+    <row r="119" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A119" s="3">
         <v>118</v>
       </c>
@@ -6284,7 +6278,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="18.75" customHeight="1">
+    <row r="120" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A120" s="3">
         <v>119</v>
       </c>
@@ -6307,7 +6301,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="121" spans="1:7" ht="18.75" customHeight="1">
+    <row r="121" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A121" s="3">
         <v>120</v>
       </c>
@@ -6330,7 +6324,7 @@
         <v>2007</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="18.75" customHeight="1">
+    <row r="122" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A122" s="3">
         <v>121</v>
       </c>
@@ -6353,7 +6347,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="18.75" customHeight="1">
+    <row r="123" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A123" s="3">
         <v>122</v>
       </c>
@@ -6376,7 +6370,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="124" spans="1:7" ht="18.75" customHeight="1">
+    <row r="124" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A124" s="3">
         <v>123</v>
       </c>
@@ -6399,7 +6393,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="125" spans="1:7" ht="18.75" customHeight="1">
+    <row r="125" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A125" s="3">
         <v>124</v>
       </c>
@@ -6422,7 +6416,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="18.75" customHeight="1">
+    <row r="126" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A126" s="3">
         <v>125</v>
       </c>
@@ -6445,7 +6439,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="18.75" customHeight="1">
+    <row r="127" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A127" s="3">
         <v>126</v>
       </c>
@@ -6468,7 +6462,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="18.75" customHeight="1">
+    <row r="128" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A128" s="3">
         <v>127</v>
       </c>
@@ -6491,7 +6485,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="129" spans="1:7" ht="18.75" customHeight="1">
+    <row r="129" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A129" s="3">
         <v>128</v>
       </c>
@@ -6514,7 +6508,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="130" spans="1:7" ht="18.75" customHeight="1">
+    <row r="130" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A130" s="3">
         <v>129</v>
       </c>
@@ -6537,7 +6531,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="131" spans="1:7" ht="18.75" customHeight="1">
+    <row r="131" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A131" s="3">
         <v>130</v>
       </c>
@@ -6560,7 +6554,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="132" spans="1:7" ht="18.75" customHeight="1">
+    <row r="132" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A132" s="3">
         <v>131</v>
       </c>
@@ -6583,7 +6577,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="133" spans="1:7" ht="18.75" customHeight="1">
+    <row r="133" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A133" s="3">
         <v>132</v>
       </c>
@@ -6606,7 +6600,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="134" spans="1:7" ht="18.75" customHeight="1">
+    <row r="134" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A134" s="3">
         <v>133</v>
       </c>
@@ -6629,7 +6623,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="18.75" customHeight="1">
+    <row r="135" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A135" s="3">
         <v>134</v>
       </c>
@@ -6652,7 +6646,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="136" spans="1:7" ht="18.75" customHeight="1">
+    <row r="136" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A136" s="3">
         <v>135</v>
       </c>
@@ -6675,7 +6669,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="137" spans="1:7" ht="18.75" customHeight="1">
+    <row r="137" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A137" s="3">
         <v>136</v>
       </c>
@@ -6698,7 +6692,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="138" spans="1:7" ht="18.75" customHeight="1">
+    <row r="138" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A138" s="3">
         <v>137</v>
       </c>
@@ -6721,7 +6715,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="139" spans="1:7" ht="18.75" customHeight="1">
+    <row r="139" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A139" s="3">
         <v>138</v>
       </c>
@@ -6744,7 +6738,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="140" spans="1:7" ht="18.75" customHeight="1">
+    <row r="140" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A140" s="3">
         <v>139</v>
       </c>
@@ -6767,7 +6761,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="18.75" customHeight="1">
+    <row r="141" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A141" s="3">
         <v>140</v>
       </c>
@@ -6790,7 +6784,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="18.75" customHeight="1">
+    <row r="142" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A142" s="3">
         <v>141</v>
       </c>
@@ -6813,7 +6807,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="143" spans="1:7" ht="18.75" customHeight="1">
+    <row r="143" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A143" s="3">
         <v>142</v>
       </c>
@@ -6836,7 +6830,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="144" spans="1:7" ht="18.75" customHeight="1">
+    <row r="144" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A144" s="3">
         <v>143</v>
       </c>
@@ -6859,7 +6853,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="145" spans="1:7" ht="18.75" customHeight="1">
+    <row r="145" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A145" s="3">
         <v>144</v>
       </c>
@@ -6882,7 +6876,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="18.75" customHeight="1">
+    <row r="146" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A146" s="3">
         <v>145</v>
       </c>
@@ -6905,7 +6899,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="18.75" customHeight="1">
+    <row r="147" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A147" s="3">
         <v>146</v>
       </c>
@@ -6928,7 +6922,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="18.75" customHeight="1">
+    <row r="148" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A148" s="3">
         <v>147</v>
       </c>
@@ -6951,7 +6945,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="18.75" customHeight="1">
+    <row r="149" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A149" s="3">
         <v>148</v>
       </c>
@@ -6974,7 +6968,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="18.75" customHeight="1">
+    <row r="150" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A150" s="3">
         <v>149</v>
       </c>
@@ -6997,7 +6991,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="18.75" customHeight="1">
+    <row r="151" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A151" s="3">
         <v>150</v>
       </c>
@@ -7020,7 +7014,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="18.75" customHeight="1">
+    <row r="152" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A152" s="3">
         <v>151</v>
       </c>
@@ -7043,7 +7037,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="18.75" customHeight="1">
+    <row r="153" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A153" s="3">
         <v>152</v>
       </c>
@@ -7066,7 +7060,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="18.75" customHeight="1">
+    <row r="154" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A154" s="3">
         <v>153</v>
       </c>
@@ -7089,7 +7083,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="18.75" customHeight="1">
+    <row r="155" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A155" s="3">
         <v>154</v>
       </c>
@@ -7112,7 +7106,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="18.75" customHeight="1">
+    <row r="156" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A156" s="3">
         <v>155</v>
       </c>
@@ -7135,7 +7129,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="18.75" customHeight="1">
+    <row r="157" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A157" s="3">
         <v>156</v>
       </c>
@@ -7158,7 +7152,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="18.75" customHeight="1">
+    <row r="158" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A158" s="3">
         <v>157</v>
       </c>
@@ -7181,7 +7175,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="18.75" customHeight="1">
+    <row r="159" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A159" s="3">
         <v>158</v>
       </c>
@@ -7204,7 +7198,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="18.75" customHeight="1">
+    <row r="160" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A160" s="3">
         <v>159</v>
       </c>
@@ -7227,7 +7221,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="18.75" customHeight="1">
+    <row r="161" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A161" s="3">
         <v>160</v>
       </c>
@@ -7250,7 +7244,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="18.75" customHeight="1">
+    <row r="162" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A162" s="3">
         <v>161</v>
       </c>
@@ -7273,7 +7267,7 @@
         <v>2009</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="18.75" customHeight="1">
+    <row r="163" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A163" s="3">
         <v>162</v>
       </c>
@@ -7296,7 +7290,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="18.75" customHeight="1">
+    <row r="164" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A164" s="3">
         <v>163</v>
       </c>
@@ -7319,7 +7313,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="18.75" customHeight="1">
+    <row r="165" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A165" s="3">
         <v>164</v>
       </c>
@@ -7342,7 +7336,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="18.75" customHeight="1">
+    <row r="166" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A166" s="3">
         <v>165</v>
       </c>
@@ -7365,7 +7359,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="18.75" customHeight="1">
+    <row r="167" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A167" s="3">
         <v>166</v>
       </c>
@@ -7388,7 +7382,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="18.75" customHeight="1">
+    <row r="168" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A168" s="3">
         <v>167</v>
       </c>
@@ -7411,7 +7405,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="169" spans="1:7" ht="18.75" customHeight="1">
+    <row r="169" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A169" s="3">
         <v>168</v>
       </c>
@@ -7434,7 +7428,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="170" spans="1:7" ht="18.75" customHeight="1">
+    <row r="170" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A170" s="3">
         <v>169</v>
       </c>
@@ -7457,7 +7451,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="171" spans="1:7" ht="18.75" customHeight="1">
+    <row r="171" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A171" s="3">
         <v>170</v>
       </c>

</xml_diff>